<commit_message>
Initial commit of Java project structure
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5688" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5688"/>
   </bookViews>
   <sheets>
-    <sheet name="Products" sheetId="1" r:id="rId1"/>
-    <sheet name="Checkout" sheetId="2" r:id="rId2"/>
+    <sheet name="ProductData" sheetId="1" r:id="rId1"/>
+    <sheet name="CheckoutData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,63 +25,87 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>Product Name</t>
-  </si>
-  <si>
-    <t>Size</t>
-  </si>
-  <si>
-    <t>Expected Price</t>
-  </si>
-  <si>
-    <t>T-shirt</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>M</t>
   </si>
   <si>
-    <t>$15.00</t>
-  </si>
-  <si>
-    <t>Jacket</t>
-  </si>
-  <si>
     <t>L</t>
   </si>
   <si>
-    <t>$40.00</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>Zip</t>
-  </si>
-  <si>
-    <t>John Doe</t>
-  </si>
-  <si>
-    <t>123 Automation St</t>
-  </si>
-  <si>
-    <t>Testville</t>
-  </si>
-  <si>
-    <t>Jane Smith</t>
-  </si>
-  <si>
-    <t>456 Selenium Ave</t>
-  </si>
-  <si>
-    <t>QA City</t>
+    <t xml:space="preserve">Email </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phone </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address </t>
+  </si>
+  <si>
+    <t xml:space="preserve">City </t>
+  </si>
+  <si>
+    <t xml:space="preserve">State </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zip </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country </t>
+  </si>
+  <si>
+    <t>test1@example.com</t>
+  </si>
+  <si>
+    <t>test2@example.com</t>
+  </si>
+  <si>
+    <t>test3@example.com</t>
+  </si>
+  <si>
+    <t>123 Main St</t>
+  </si>
+  <si>
+    <t xml:space="preserve">456 Oak Ave </t>
+  </si>
+  <si>
+    <t>789 Pine Rd</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>San Diego</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ProductIndex </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mens_outerwear </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ladies_outerwear </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size </t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -103,10 +127,10 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
+      <sz val="8"/>
+      <color rgb="FF383A42"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -144,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -152,12 +176,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,45 +457,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
+      <c r="D5" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -487,54 +543,104 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B2" s="3">
+        <v>1234567890</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="3">
+        <v>90001</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="B3" s="3">
+        <v>9876543210</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="3">
+        <v>94102</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="B4" s="3">
+        <v>5551234567</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="3">
-        <v>12345</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="3">
-        <v>67890</v>
+      <c r="F4" s="3">
+        <v>92101</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial commit of my project
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kvina\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5688"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12300" windowHeight="3300"/>
   </bookViews>
   <sheets>
     <sheet name="ProductData" sheetId="1" r:id="rId1"/>
     <sheet name="CheckoutData" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:L9"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -460,7 +456,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>